<commit_message>
#20: Confirms t-test stability for gender by age groups w. updated data
</commit_message>
<xml_diff>
--- a/raw/Raw and Age-Adjusted National Mortality Rates by Gender per 1M (2007 - 2020).xlsx
+++ b/raw/Raw and Age-Adjusted National Mortality Rates by Gender per 1M (2007 - 2020).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernair-desai/Desktop/IndRes/CJD_Epi/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C79902B1-ACBF-C043-AC7A-33CBA6EBC168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF8B2C8-7BE0-2645-8C96-DA08BB2AFD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3120" yWindow="760" windowWidth="27240" windowHeight="16440" xr2:uid="{76FFD262-DFFE-874F-8847-8BD305C51152}"/>
+    <workbookView xWindow="4480" yWindow="4300" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{76FFD262-DFFE-874F-8847-8BD305C51152}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality Rates" sheetId="1" r:id="rId1"/>
@@ -657,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DED045-55C7-2E44-933B-228F0388AF95}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -2575,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB96669-47DC-9F46-994A-A02BE947DB4E}">
   <dimension ref="A1:A68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2819,107 +2819,107 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>81</v>
       </c>

</xml_diff>